<commit_message>
atualizacao BD part 2
</commit_message>
<xml_diff>
--- a/Bd/Dicionário_Dados_Microstart.xlsx
+++ b/Bd/Dicionário_Dados_Microstart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24722"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Criação de Sites\BRMODELOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\MicroStart\Bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{7C452921-5B1F-43E8-90E1-088B49E4CD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B84E25-A5F1-4E27-8A0D-96001F3F050C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD559922-3DBC-44C5-92B1-F9E3E2F4DEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{F97B2F44-631C-4B1A-B8A0-EC6BCA9D2207}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F97B2F44-631C-4B1A-B8A0-EC6BCA9D2207}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="84">
   <si>
     <t>DICIONÁRIO DE DADOS</t>
   </si>
@@ -69,9 +69,6 @@
     <t>PK/FK/NOT NULL/DEFAULT</t>
   </si>
   <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>REGISTRA AS VENDAS FEITAS PARA O CLIENTE</t>
   </si>
   <si>
-    <t>CODIGO_CLIE</t>
-  </si>
-  <si>
     <t>CODIGO_PAG</t>
   </si>
   <si>
@@ -265,13 +259,40 @@
   </si>
   <si>
     <t>ARMAZENA AS TRANSPORTADORAS</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>SENHA</t>
+  </si>
+  <si>
+    <t>CODIGO_TEL</t>
+  </si>
+  <si>
+    <t>CODIGO_CON_END_CLI</t>
+  </si>
+  <si>
+    <t>CODIGO_CON_END_FORN</t>
+  </si>
+  <si>
+    <t>CODIGO_TEL_FORN</t>
+  </si>
+  <si>
+    <t>CODIGO_FORN_PRODUTO</t>
+  </si>
+  <si>
+    <t>CODIGO_ITEM_VENDA</t>
+  </si>
+  <si>
+    <t>CODIGO_REGISTRO_VENDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +312,27 @@
       <color theme="1"/>
       <name val="Algerian"/>
       <family val="5"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -513,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -617,6 +659,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +692,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -933,13 +990,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25B40A3-EAC1-4FDA-A215-91A86A7DB5E8}">
   <dimension ref="A1:P195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190:G190"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L188" sqref="L188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" thickTop="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -957,7 +1014,7 @@
       <c r="O1" s="8"/>
       <c r="P1" s="9"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -971,8 +1028,8 @@
       <c r="O2" s="11"/>
       <c r="P2" s="12"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickTop="1"/>
-    <row r="4" spans="1:16">
+    <row r="3" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -988,7 +1045,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -1004,7 +1061,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1018,7 +1075,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1095,7 @@
       <c r="I7" s="22"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="20"/>
@@ -1050,13 +1107,13 @@
       <c r="I8" s="23"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
@@ -1065,18 +1122,18 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -1085,18 +1142,18 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
@@ -1105,38 +1162,36 @@
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="4">
-        <v>10</v>
-      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
@@ -1145,42 +1200,58 @@
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <v>50</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <v>100</v>
+      </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1190,13 +1261,13 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1206,7 +1277,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1220,7 +1291,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>7</v>
       </c>
@@ -1240,7 +1311,7 @@
       <c r="I20" s="22"/>
       <c r="J20" s="19"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
       <c r="C21" s="20"/>
@@ -1252,13 +1323,13 @@
       <c r="I21" s="23"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
@@ -1267,18 +1338,18 @@
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
@@ -1287,18 +1358,18 @@
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="24"/>
       <c r="J23" s="24"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
@@ -1307,12 +1378,12 @@
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="24"/>
@@ -1324,7 +1395,7 @@
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="24"/>
@@ -1336,7 +1407,7 @@
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="24"/>
@@ -1348,7 +1419,7 @@
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="24"/>
@@ -1360,13 +1431,13 @@
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -1376,13 +1447,13 @@
       <c r="I30" s="24"/>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -1392,7 +1463,7 @@
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1477,7 @@
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1497,7 @@
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
@@ -1438,13 +1509,13 @@
       <c r="I34" s="26"/>
       <c r="J34" s="26"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="24" t="s">
-        <v>11</v>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>78</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -1453,18 +1524,18 @@
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I35" s="24"/>
       <c r="J35" s="24"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -1473,18 +1544,18 @@
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" s="24"/>
       <c r="J36" s="24"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -1493,18 +1564,18 @@
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="24"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -1513,18 +1584,18 @@
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -1533,18 +1604,18 @@
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
@@ -1554,13 +1625,13 @@
       <c r="I41" s="24"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
@@ -1570,7 +1641,7 @@
       <c r="I42" s="24"/>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>6</v>
       </c>
@@ -1584,7 +1655,7 @@
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>7</v>
       </c>
@@ -1604,7 +1675,7 @@
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="26"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -1616,13 +1687,13 @@
       <c r="I45" s="26"/>
       <c r="J45" s="26"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
@@ -1631,18 +1702,18 @@
       </c>
       <c r="G46" s="24"/>
       <c r="H46" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I46" s="24"/>
       <c r="J46" s="24"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
@@ -1651,18 +1722,18 @@
       </c>
       <c r="G47" s="24"/>
       <c r="H47" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I47" s="24"/>
       <c r="J47" s="24"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
@@ -1671,18 +1742,18 @@
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I48" s="24"/>
       <c r="J48" s="24"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
@@ -1691,18 +1762,18 @@
       </c>
       <c r="G49" s="24"/>
       <c r="H49" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I49" s="24"/>
       <c r="J49" s="24"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
@@ -1711,18 +1782,18 @@
       </c>
       <c r="G50" s="24"/>
       <c r="H50" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I50" s="24"/>
       <c r="J50" s="24"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
@@ -1731,18 +1802,18 @@
       </c>
       <c r="G51" s="24"/>
       <c r="H51" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I51" s="24"/>
       <c r="J51" s="24"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
@@ -1751,22 +1822,22 @@
       </c>
       <c r="G52" s="24"/>
       <c r="H52" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I52" s="24"/>
       <c r="J52" s="24"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="25"/>
       <c r="B53" s="25"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1776,13 +1847,13 @@
       <c r="I54" s="6"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -1792,7 +1863,7 @@
       <c r="I55" s="6"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>6</v>
       </c>
@@ -1806,7 +1877,7 @@
       <c r="I56" s="16"/>
       <c r="J56" s="17"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1897,7 @@
       <c r="I57" s="22"/>
       <c r="J57" s="19"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
       <c r="B58" s="21"/>
       <c r="C58" s="20"/>
@@ -1838,13 +1909,13 @@
       <c r="I58" s="23"/>
       <c r="J58" s="21"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="5"/>
@@ -1853,18 +1924,18 @@
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I59" s="6"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
@@ -1873,18 +1944,18 @@
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
@@ -1893,18 +1964,18 @@
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="5"/>
@@ -1913,18 +1984,18 @@
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I62" s="6"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="5"/>
@@ -1933,42 +2004,58 @@
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I63" s="6"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="4"/>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="B64" s="5"/>
-      <c r="C64" s="4"/>
+      <c r="C64" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D64" s="6"/>
       <c r="E64" s="5"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="4">
+        <v>50</v>
+      </c>
       <c r="G64" s="5"/>
-      <c r="H64" s="4"/>
+      <c r="H64" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I64" s="6"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="4"/>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B65" s="5"/>
-      <c r="C65" s="4"/>
+      <c r="C65" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D65" s="6"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="4">
+        <v>100</v>
+      </c>
       <c r="G65" s="5"/>
-      <c r="H65" s="4"/>
+      <c r="H65" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I65" s="6"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -1978,13 +2065,13 @@
       <c r="I67" s="6"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
@@ -1994,7 +2081,7 @@
       <c r="I68" s="6"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>6</v>
       </c>
@@ -2008,7 +2095,7 @@
       <c r="I69" s="16"/>
       <c r="J69" s="17"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>7</v>
       </c>
@@ -2028,7 +2115,7 @@
       <c r="I70" s="22"/>
       <c r="J70" s="19"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="20"/>
       <c r="B71" s="21"/>
       <c r="C71" s="20"/>
@@ -2040,13 +2127,13 @@
       <c r="I71" s="23"/>
       <c r="J71" s="21"/>
     </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="41"/>
+      <c r="C72" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
@@ -2055,18 +2142,18 @@
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="5"/>
@@ -2075,18 +2162,18 @@
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="5"/>
@@ -2095,18 +2182,18 @@
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="5"/>
@@ -2115,18 +2202,18 @@
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -2135,12 +2222,12 @@
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I76" s="6"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="4"/>
@@ -2152,7 +2239,7 @@
       <c r="I77" s="6"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
       <c r="C78" s="4"/>
@@ -2164,13 +2251,13 @@
       <c r="I78" s="6"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
@@ -2180,13 +2267,13 @@
       <c r="I80" s="6"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B81" s="14"/>
       <c r="C81" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
@@ -2196,7 +2283,7 @@
       <c r="I81" s="6"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>6</v>
       </c>
@@ -2210,7 +2297,7 @@
       <c r="I82" s="16"/>
       <c r="J82" s="17"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
         <v>7</v>
       </c>
@@ -2230,7 +2317,7 @@
       <c r="I83" s="22"/>
       <c r="J83" s="19"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="B84" s="21"/>
       <c r="C84" s="20"/>
@@ -2242,13 +2329,13 @@
       <c r="I84" s="23"/>
       <c r="J84" s="21"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
@@ -2257,18 +2344,18 @@
       </c>
       <c r="G85" s="5"/>
       <c r="H85" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I85" s="6"/>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
@@ -2277,18 +2364,18 @@
       </c>
       <c r="G86" s="5"/>
       <c r="H86" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
@@ -2297,12 +2384,12 @@
       </c>
       <c r="G87" s="5"/>
       <c r="H87" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I87" s="6"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="4"/>
@@ -2314,7 +2401,7 @@
       <c r="I88" s="6"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="4"/>
@@ -2326,7 +2413,7 @@
       <c r="I89" s="6"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="4"/>
@@ -2338,7 +2425,7 @@
       <c r="I90" s="6"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="4"/>
@@ -2350,13 +2437,13 @@
       <c r="I91" s="6"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
@@ -2366,13 +2453,13 @@
       <c r="I93" s="6"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
@@ -2382,7 +2469,7 @@
       <c r="I94" s="6"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
         <v>6</v>
       </c>
@@ -2396,7 +2483,7 @@
       <c r="I95" s="16"/>
       <c r="J95" s="17"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
         <v>7</v>
       </c>
@@ -2416,7 +2503,7 @@
       <c r="I96" s="22"/>
       <c r="J96" s="19"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
       <c r="B97" s="21"/>
       <c r="C97" s="20"/>
@@ -2428,13 +2515,13 @@
       <c r="I97" s="23"/>
       <c r="J97" s="21"/>
     </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B98" s="5"/>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" s="41"/>
       <c r="C98" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D98" s="6"/>
       <c r="E98" s="5"/>
@@ -2443,18 +2530,18 @@
       </c>
       <c r="G98" s="5"/>
       <c r="H98" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I98" s="6"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D99" s="6"/>
       <c r="E99" s="5"/>
@@ -2463,18 +2550,18 @@
       </c>
       <c r="G99" s="5"/>
       <c r="H99" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I99" s="6"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="5"/>
@@ -2483,12 +2570,12 @@
       </c>
       <c r="G100" s="5"/>
       <c r="H100" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I100" s="6"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="4"/>
@@ -2500,7 +2587,7 @@
       <c r="I101" s="6"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
       <c r="C102" s="4"/>
@@ -2512,7 +2599,7 @@
       <c r="I102" s="6"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="4"/>
@@ -2524,7 +2611,7 @@
       <c r="I103" s="6"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
       <c r="C104" s="4"/>
@@ -2536,13 +2623,13 @@
       <c r="I104" s="6"/>
       <c r="J104" s="5"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
@@ -2552,13 +2639,13 @@
       <c r="I106" s="6"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
@@ -2568,7 +2655,7 @@
       <c r="I107" s="6"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>6</v>
       </c>
@@ -2582,7 +2669,7 @@
       <c r="I108" s="16"/>
       <c r="J108" s="17"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
         <v>7</v>
       </c>
@@ -2602,7 +2689,7 @@
       <c r="I109" s="22"/>
       <c r="J109" s="19"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="20"/>
@@ -2614,13 +2701,13 @@
       <c r="I110" s="23"/>
       <c r="J110" s="21"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B111" s="5"/>
       <c r="C111" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="5"/>
@@ -2629,18 +2716,18 @@
       </c>
       <c r="G111" s="5"/>
       <c r="H111" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I111" s="6"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="5"/>
@@ -2649,18 +2736,18 @@
       </c>
       <c r="G112" s="5"/>
       <c r="H112" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I112" s="6"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="5"/>
@@ -2669,18 +2756,18 @@
       </c>
       <c r="G113" s="5"/>
       <c r="H113" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="5"/>
@@ -2689,18 +2776,18 @@
       </c>
       <c r="G114" s="5"/>
       <c r="H114" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I114" s="6"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B115" s="5"/>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B115" s="39"/>
       <c r="C115" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="5"/>
@@ -2709,18 +2796,18 @@
       </c>
       <c r="G115" s="5"/>
       <c r="H115" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I115" s="6"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B116" s="5"/>
       <c r="C116" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="5"/>
@@ -2729,18 +2816,18 @@
       </c>
       <c r="G116" s="5"/>
       <c r="H116" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="5"/>
@@ -2749,18 +2836,18 @@
       </c>
       <c r="G117" s="5"/>
       <c r="H117" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I117" s="6"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
@@ -2770,13 +2857,13 @@
       <c r="I119" s="6"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
@@ -2786,7 +2873,7 @@
       <c r="I120" s="6"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
         <v>6</v>
       </c>
@@ -2800,7 +2887,7 @@
       <c r="I121" s="16"/>
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
         <v>7</v>
       </c>
@@ -2820,7 +2907,7 @@
       <c r="I122" s="22"/>
       <c r="J122" s="19"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="21"/>
       <c r="C123" s="20"/>
@@ -2832,13 +2919,13 @@
       <c r="I123" s="23"/>
       <c r="J123" s="21"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="5"/>
@@ -2847,18 +2934,18 @@
       </c>
       <c r="G124" s="5"/>
       <c r="H124" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I124" s="6"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B125" s="5"/>
       <c r="C125" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="5"/>
@@ -2867,12 +2954,12 @@
       </c>
       <c r="G125" s="5"/>
       <c r="H125" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I125" s="6"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="5"/>
       <c r="C126" s="4"/>
@@ -2884,7 +2971,7 @@
       <c r="I126" s="6"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="5"/>
       <c r="C127" s="4"/>
@@ -2896,7 +2983,7 @@
       <c r="I127" s="6"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="5"/>
       <c r="C128" s="4"/>
@@ -2908,7 +2995,7 @@
       <c r="I128" s="6"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="5"/>
       <c r="C129" s="4"/>
@@ -2920,7 +3007,7 @@
       <c r="I129" s="6"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="5"/>
       <c r="C130" s="4"/>
@@ -2932,13 +3019,13 @@
       <c r="I130" s="6"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B132" s="14"/>
       <c r="C132" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
@@ -2948,13 +3035,13 @@
       <c r="I132" s="6"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B133" s="14"/>
       <c r="C133" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
@@ -2964,7 +3051,7 @@
       <c r="I133" s="6"/>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
         <v>6</v>
       </c>
@@ -2978,7 +3065,7 @@
       <c r="I134" s="16"/>
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="18" t="s">
         <v>7</v>
       </c>
@@ -2998,7 +3085,7 @@
       <c r="I135" s="22"/>
       <c r="J135" s="19"/>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="21"/>
       <c r="C136" s="20"/>
@@ -3010,13 +3097,13 @@
       <c r="I136" s="23"/>
       <c r="J136" s="21"/>
     </row>
-    <row r="137" spans="1:10">
-      <c r="A137" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B137" s="5"/>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B137" s="39"/>
       <c r="C137" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="5"/>
@@ -3025,18 +3112,18 @@
       </c>
       <c r="G137" s="5"/>
       <c r="H137" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I137" s="6"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="5"/>
@@ -3045,12 +3132,12 @@
       </c>
       <c r="G138" s="5"/>
       <c r="H138" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I138" s="6"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="5"/>
       <c r="C139" s="4"/>
@@ -3062,7 +3149,7 @@
       <c r="I139" s="6"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="5"/>
       <c r="C140" s="4"/>
@@ -3074,7 +3161,7 @@
       <c r="I140" s="6"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="5"/>
       <c r="C141" s="4"/>
@@ -3086,7 +3173,7 @@
       <c r="I141" s="6"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="5"/>
       <c r="C142" s="4"/>
@@ -3098,7 +3185,7 @@
       <c r="I142" s="6"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="5"/>
       <c r="C143" s="4"/>
@@ -3110,13 +3197,13 @@
       <c r="I143" s="6"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="6"/>
@@ -3126,13 +3213,13 @@
       <c r="I145" s="6"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="6"/>
@@ -3142,7 +3229,7 @@
       <c r="I146" s="6"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
         <v>6</v>
       </c>
@@ -3156,7 +3243,7 @@
       <c r="I147" s="16"/>
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="18" t="s">
         <v>7</v>
       </c>
@@ -3176,7 +3263,7 @@
       <c r="I148" s="22"/>
       <c r="J148" s="19"/>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="20"/>
       <c r="B149" s="21"/>
       <c r="C149" s="20"/>
@@ -3188,13 +3275,13 @@
       <c r="I149" s="23"/>
       <c r="J149" s="21"/>
     </row>
-    <row r="150" spans="1:10">
-      <c r="A150" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B150" s="5"/>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B150" s="39"/>
       <c r="C150" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="5"/>
@@ -3203,18 +3290,18 @@
       </c>
       <c r="G150" s="5"/>
       <c r="H150" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I150" s="6"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B151" s="5"/>
       <c r="C151" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="5"/>
@@ -3223,18 +3310,18 @@
       </c>
       <c r="G151" s="5"/>
       <c r="H151" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I151" s="6"/>
       <c r="J151" s="5"/>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B152" s="5"/>
       <c r="C152" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="5"/>
@@ -3243,18 +3330,18 @@
       </c>
       <c r="G152" s="5"/>
       <c r="H152" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I152" s="6"/>
       <c r="J152" s="5"/>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B153" s="5"/>
       <c r="C153" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="5"/>
@@ -3263,18 +3350,18 @@
       </c>
       <c r="G153" s="5"/>
       <c r="H153" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I153" s="6"/>
       <c r="J153" s="5"/>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B154" s="5"/>
       <c r="C154" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="5"/>
@@ -3283,12 +3370,12 @@
       </c>
       <c r="G154" s="5"/>
       <c r="H154" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I154" s="6"/>
       <c r="J154" s="5"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
       <c r="C155" s="4"/>
@@ -3300,7 +3387,7 @@
       <c r="I155" s="6"/>
       <c r="J155" s="5"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
       <c r="C156" s="4"/>
@@ -3312,13 +3399,13 @@
       <c r="I156" s="6"/>
       <c r="J156" s="5"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B158" s="14"/>
       <c r="C158" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
@@ -3328,13 +3415,13 @@
       <c r="I158" s="6"/>
       <c r="J158" s="5"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D159" s="6"/>
       <c r="E159" s="6"/>
@@ -3344,7 +3431,7 @@
       <c r="I159" s="6"/>
       <c r="J159" s="5"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
         <v>6</v>
       </c>
@@ -3358,7 +3445,7 @@
       <c r="I160" s="16"/>
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="18" t="s">
         <v>7</v>
       </c>
@@ -3378,7 +3465,7 @@
       <c r="I161" s="22"/>
       <c r="J161" s="19"/>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="21"/>
       <c r="C162" s="20"/>
@@ -3390,13 +3477,13 @@
       <c r="I162" s="23"/>
       <c r="J162" s="21"/>
     </row>
-    <row r="163" spans="1:10">
-      <c r="A163" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B163" s="5"/>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B163" s="41"/>
       <c r="C163" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D163" s="6"/>
       <c r="E163" s="5"/>
@@ -3405,18 +3492,18 @@
       </c>
       <c r="G163" s="5"/>
       <c r="H163" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I163" s="6"/>
       <c r="J163" s="5"/>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D164" s="6"/>
       <c r="E164" s="5"/>
@@ -3425,18 +3512,18 @@
       </c>
       <c r="G164" s="5"/>
       <c r="H164" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I164" s="6"/>
       <c r="J164" s="5"/>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D165" s="6"/>
       <c r="E165" s="5"/>
@@ -3445,18 +3532,18 @@
       </c>
       <c r="G165" s="5"/>
       <c r="H165" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I165" s="6"/>
       <c r="J165" s="5"/>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D166" s="6"/>
       <c r="E166" s="5"/>
@@ -3465,18 +3552,18 @@
       </c>
       <c r="G166" s="5"/>
       <c r="H166" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I166" s="6"/>
       <c r="J166" s="5"/>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D167" s="6"/>
       <c r="E167" s="5"/>
@@ -3485,12 +3572,12 @@
       </c>
       <c r="G167" s="5"/>
       <c r="H167" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I167" s="6"/>
       <c r="J167" s="5"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
       <c r="C168" s="4"/>
@@ -3502,7 +3589,7 @@
       <c r="I168" s="6"/>
       <c r="J168" s="5"/>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
       <c r="C169" s="4"/>
@@ -3514,13 +3601,13 @@
       <c r="I169" s="6"/>
       <c r="J169" s="5"/>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B171" s="14"/>
       <c r="C171" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="6"/>
@@ -3530,13 +3617,13 @@
       <c r="I171" s="6"/>
       <c r="J171" s="5"/>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B172" s="14"/>
       <c r="C172" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="6"/>
@@ -3546,7 +3633,7 @@
       <c r="I172" s="6"/>
       <c r="J172" s="5"/>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="15" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3647,7 @@
       <c r="I173" s="16"/>
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
         <v>7</v>
       </c>
@@ -3580,7 +3667,7 @@
       <c r="I174" s="22"/>
       <c r="J174" s="19"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="21"/>
       <c r="C175" s="20"/>
@@ -3592,13 +3679,13 @@
       <c r="I175" s="23"/>
       <c r="J175" s="21"/>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D176" s="6"/>
       <c r="E176" s="5"/>
@@ -3607,18 +3694,18 @@
       </c>
       <c r="G176" s="5"/>
       <c r="H176" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I176" s="6"/>
       <c r="J176" s="5"/>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D177" s="6"/>
       <c r="E177" s="5"/>
@@ -3627,12 +3714,12 @@
       </c>
       <c r="G177" s="5"/>
       <c r="H177" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I177" s="6"/>
       <c r="J177" s="5"/>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
       <c r="C178" s="4"/>
@@ -3644,7 +3731,7 @@
       <c r="I178" s="6"/>
       <c r="J178" s="5"/>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
       <c r="C179" s="4"/>
@@ -3656,7 +3743,7 @@
       <c r="I179" s="6"/>
       <c r="J179" s="5"/>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
       <c r="C180" s="4"/>
@@ -3668,7 +3755,7 @@
       <c r="I180" s="6"/>
       <c r="J180" s="5"/>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
       <c r="C181" s="4"/>
@@ -3680,7 +3767,7 @@
       <c r="I181" s="6"/>
       <c r="J181" s="5"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
       <c r="C182" s="4"/>
@@ -3692,13 +3779,13 @@
       <c r="I182" s="6"/>
       <c r="J182" s="5"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B184" s="14"/>
       <c r="C184" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
@@ -3708,13 +3795,13 @@
       <c r="I184" s="6"/>
       <c r="J184" s="5"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B185" s="14"/>
       <c r="C185" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
@@ -3724,7 +3811,7 @@
       <c r="I185" s="6"/>
       <c r="J185" s="5"/>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="15" t="s">
         <v>6</v>
       </c>
@@ -3738,7 +3825,7 @@
       <c r="I186" s="16"/>
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="18" t="s">
         <v>7</v>
       </c>
@@ -3758,7 +3845,7 @@
       <c r="I187" s="22"/>
       <c r="J187" s="19"/>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="20"/>
       <c r="B188" s="21"/>
       <c r="C188" s="20"/>
@@ -3770,13 +3857,13 @@
       <c r="I188" s="23"/>
       <c r="J188" s="21"/>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B189" s="5"/>
       <c r="C189" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D189" s="6"/>
       <c r="E189" s="5"/>
@@ -3785,18 +3872,18 @@
       </c>
       <c r="G189" s="5"/>
       <c r="H189" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I189" s="6"/>
       <c r="J189" s="5"/>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B190" s="5"/>
       <c r="C190" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D190" s="6"/>
       <c r="E190" s="5"/>
@@ -3805,12 +3892,12 @@
       </c>
       <c r="G190" s="5"/>
       <c r="H190" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I190" s="6"/>
       <c r="J190" s="5"/>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
       <c r="C191" s="4"/>
@@ -3822,7 +3909,7 @@
       <c r="I191" s="6"/>
       <c r="J191" s="5"/>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
       <c r="C192" s="4"/>
@@ -3834,7 +3921,7 @@
       <c r="I192" s="6"/>
       <c r="J192" s="5"/>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
       <c r="C193" s="4"/>
@@ -3846,7 +3933,7 @@
       <c r="I193" s="6"/>
       <c r="J193" s="5"/>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
       <c r="C194" s="4"/>
@@ -3858,7 +3945,7 @@
       <c r="I194" s="6"/>
       <c r="J194" s="5"/>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
       <c r="C195" s="4"/>
@@ -3996,9 +4083,6 @@
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="F49:G49"/>
@@ -4008,11 +4092,8 @@
     <mergeCell ref="F50:G50"/>
     <mergeCell ref="H50:J50"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
     <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
     <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="F59:G59"/>
@@ -4030,6 +4111,12 @@
     <mergeCell ref="C57:E58"/>
     <mergeCell ref="F57:G58"/>
     <mergeCell ref="H57:J58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="F63:G63"/>
@@ -4428,21 +4515,39 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DDB387495ADE264BB39771AD5D24F372" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d63e19f649836db38f2e244908a8c9ea">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9974a67a-c558-4715-80c2-702e37bde580" xmlns:ns4="7f8111d8-83a9-48e4-a46c-3f5275a78710" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00e09ee65702c14b000aa75673fd3d4c" ns3:_="" ns4:_="">
-    <xsd:import namespace="9974a67a-c558-4715-80c2-702e37bde580"/>
-    <xsd:import namespace="7f8111d8-83a9-48e4-a46c-3f5275a78710"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011597D82AA56DB448934E2DDD468B6DF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4fa52593d49d833a167c7ff4531354e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0d879487-596d-4348-876f-f35992d12014" xmlns:ns4="b2c127de-30d0-4fad-bee6-8dd763b4fdf7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19fda2333a74ba36e378df92ad6149cc" ns3:_="" ns4:_="">
+    <xsd:import namespace="0d879487-596d-4348-876f-f35992d12014"/>
+    <xsd:import namespace="b2c127de-30d0-4fad-bee6-8dd763b4fdf7"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4450,10 +4555,41 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9974a67a-c558-4715-80c2-702e37bde580" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0d879487-596d-4348-876f-f35992d12014" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b2c127de-30d0-4fad-bee6-8dd763b4fdf7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="13" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -4472,30 +4608,16 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="14" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+    <xsd:element name="SharingHintHash" ma:index="15" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7f8111d8-83a9-48e4-a46c-3f5275a78710" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4598,29 +4720,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47EAC94C-74C4-4A98-AD7B-03FB5DB7C72C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE23ECC-EE5D-49EB-8C7F-8551E565AECB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEED03C-32A4-467A-906D-F184390723C0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEED03C-32A4-467A-906D-F184390723C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0d879487-596d-4348-876f-f35992d12014"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b2c127de-30d0-4fad-bee6-8dd763b4fdf7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE23ECC-EE5D-49EB-8C7F-8551E565AECB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DF2DDB8-DA7A-4793-BA63-BB6F8C6B77D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d879487-596d-4348-876f-f35992d12014"/>
+    <ds:schemaRef ds:uri="b2c127de-30d0-4fad-bee6-8dd763b4fdf7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>